<commit_message>
Developed e2eOrder test scripts to support test cases order_01-order_10 with action add, addOn, delete
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testCaseCriteria/testCaseCriteria_login.xlsx
+++ b/cypress/fixtures/testCaseCriteria/testCaseCriteria_login.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationexercise\cypress\fixtures\testCaseCriterial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationexercise\cypress\fixtures\testCaseCriteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72A887C-C6FF-4086-BE66-92ECEF74078D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA513A76-932B-4211-A24A-5E57DE74B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="553" firstSheet="1" activeTab="6" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
   </bookViews>
   <sheets>
     <sheet name="column_ref" sheetId="2" r:id="rId1"/>
     <sheet name="login_01" sheetId="17" r:id="rId2"/>
     <sheet name="login_02" sheetId="18" r:id="rId3"/>
     <sheet name="login_03" sheetId="19" r:id="rId4"/>
+    <sheet name="login_04" sheetId="22" r:id="rId5"/>
+    <sheet name="login_05" sheetId="20" r:id="rId6"/>
+    <sheet name="login_06" sheetId="21" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>action</t>
   </si>
@@ -83,18 +86,9 @@
     <t>login|name</t>
   </si>
   <si>
-    <t>login, signup, logout</t>
-  </si>
-  <si>
     <t>success</t>
   </si>
   <si>
-    <t>success, failed</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
@@ -105,13 +99,36 @@
   </si>
   <si>
     <t>login|result</t>
+  </si>
+  <si>
+    <t>failed-incorrect</t>
+  </si>
+  <si>
+    <t>failed-filledPassword</t>
+  </si>
+  <si>
+    <t>failed-filledEmail</t>
+  </si>
+  <si>
+    <t>automated.test2@mail.com</t>
+  </si>
+  <si>
+    <t>success
+failed-incorrect
+failed-filledPassword
+failed-filledEmail</t>
+  </si>
+  <si>
+    <t>login
+signup
+logout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,14 +140,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,11 +188,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,20 +210,37 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,16 +555,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C6351B-47AC-4A85-A3FB-088019320162}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" style="4" customWidth="1"/>
-    <col min="3" max="4" width="15.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="5" customWidth="1"/>
+    <col min="3" max="4" width="20.6328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -556,32 +581,29 @@
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="16" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>9</v>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{64537A50-09F2-4D90-9C35-EC4318CD74EA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -590,19 +612,17 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" style="9" customWidth="1"/>
-    <col min="8" max="10" width="15.6328125" style="9" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="8" customWidth="1"/>
     <col min="11" max="17" width="15.6328125" customWidth="1"/>
     <col min="18" max="19" width="25.6328125" customWidth="1"/>
     <col min="20" max="25" width="15.6328125" customWidth="1"/>
@@ -626,21 +646,102 @@
         <v>login|result</v>
       </c>
     </row>
+    <row r="2" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195EE033-E3EF-4AB8-A6E9-36A02CB90136}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="8" customWidth="1"/>
+    <col min="11" max="17" width="15.6328125" customWidth="1"/>
+    <col min="18" max="19" width="25.6328125" customWidth="1"/>
+    <col min="20" max="25" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="str" cm="1">
+        <f t="array" ref="A1:E1">column_ref!A1:E1</f>
+        <v>action</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>login|email</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>login|password</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>login|name</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>login|result</v>
+      </c>
+    </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>8</v>
+      <c r="E2" s="14" t="s">
+        <v>7</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -668,24 +769,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195EE033-E3EF-4AB8-A6E9-36A02CB90136}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F483DD-3067-4B7F-93BD-593B08243EB7}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.6328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" style="9" customWidth="1"/>
-    <col min="8" max="10" width="15.6328125" style="9" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="8" customWidth="1"/>
     <col min="11" max="17" width="15.6328125" customWidth="1"/>
     <col min="18" max="19" width="25.6328125" customWidth="1"/>
     <col min="20" max="25" width="15.6328125" customWidth="1"/>
@@ -710,20 +809,18 @@
       </c>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -751,24 +848,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F483DD-3067-4B7F-93BD-593B08243EB7}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55EA4C3-D33C-45B7-9965-6ED58AEA0BD8}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.6328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.6328125" style="9" customWidth="1"/>
-    <col min="8" max="10" width="15.6328125" style="9" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="8" customWidth="1"/>
     <col min="11" max="17" width="15.6328125" customWidth="1"/>
     <col min="18" max="19" width="25.6328125" customWidth="1"/>
     <col min="20" max="25" width="15.6328125" customWidth="1"/>
@@ -793,18 +888,18 @@
       </c>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>11</v>
+      <c r="A2" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
@@ -830,4 +925,158 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CFBED9-18E4-48C0-BFB2-8258F775FD4D}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="8" customWidth="1"/>
+    <col min="11" max="17" width="15.6328125" customWidth="1"/>
+    <col min="18" max="19" width="25.6328125" customWidth="1"/>
+    <col min="20" max="25" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="str" cm="1">
+        <f t="array" ref="A1:E1">column_ref!A1:E1</f>
+        <v>action</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>login|email</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>login|password</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>login|name</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>login|result</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5476C5D0-8A16-4092-B140-CED632B43AC3}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.6328125" style="5" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="8" customWidth="1"/>
+    <col min="8" max="10" width="15.6328125" style="8" customWidth="1"/>
+    <col min="11" max="17" width="15.6328125" customWidth="1"/>
+    <col min="18" max="19" width="25.6328125" customWidth="1"/>
+    <col min="20" max="25" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="str" cm="1">
+        <f t="array" ref="A1:E1">column_ref!A1:E1</f>
+        <v>action</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>login|email</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>login|password</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>login|name</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>login|result</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>